<commit_message>
Updated front_end.py to include as much functionality as possible.
</commit_message>
<xml_diff>
--- a/FailureTable.xlsx
+++ b/FailureTable.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4d965ff5125c3e04/University/Year 1 Sem 2/Software QA/SQA Project/SQA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1A19906C-396F-4516-B957-E8AC86749972}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="13" documentId="8_{1A19906C-396F-4516-B957-E8AC86749972}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5B04789F-4D01-4A6B-8B04-A7F7748C3593}"/>
   <bookViews>
-    <workbookView xWindow="2496" yWindow="2460" windowWidth="23040" windowHeight="14688" xr2:uid="{84DE182B-CA28-43A4-8BC3-90ADADE2CD3E}"/>
+    <workbookView xWindow="18756" yWindow="3984" windowWidth="23040" windowHeight="14688" xr2:uid="{84DE182B-CA28-43A4-8BC3-90ADADE2CD3E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="8">
   <si>
     <t>Test Name</t>
   </si>
@@ -47,10 +47,19 @@
     <t>Failure Description</t>
   </si>
   <si>
-    <t>Cause of Error</t>
-  </si>
-  <si>
     <t>Fix Implemented</t>
+  </si>
+  <si>
+    <t>Login</t>
+  </si>
+  <si>
+    <t>Data validation</t>
+  </si>
+  <si>
+    <t>No check to prevent multiple logins</t>
+  </si>
+  <si>
+    <t>No restriction for admin-only transactions with standard login</t>
   </si>
 </sst>
 </file>
@@ -422,21 +431,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78A7481D-5A8F-4A12-81BF-F0F307BBE9C7}">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12.77734375" customWidth="1"/>
-    <col min="2" max="3" width="17.88671875" customWidth="1"/>
-    <col min="4" max="4" width="13.6640625" customWidth="1"/>
+    <col min="2" max="2" width="17.88671875" customWidth="1"/>
+    <col min="3" max="3" width="49.21875" customWidth="1"/>
+    <col min="4" max="4" width="27.88671875" customWidth="1"/>
     <col min="5" max="5" width="14.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -449,7 +459,31 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Okay now it works
</commit_message>
<xml_diff>
--- a/FailureTable.xlsx
+++ b/FailureTable.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4d965ff5125c3e04/University/Year 1 Sem 2/Software QA/SQA Project/SQA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="13" documentId="8_{1A19906C-396F-4516-B957-E8AC86749972}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5B04789F-4D01-4A6B-8B04-A7F7748C3593}"/>
+  <xr:revisionPtr revIDLastSave="134" documentId="8_{1A19906C-396F-4516-B957-E8AC86749972}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{34678FBE-2C41-4E9A-BE12-E11B5E1DF877}"/>
   <bookViews>
-    <workbookView xWindow="18756" yWindow="3984" windowWidth="23040" windowHeight="14688" xr2:uid="{84DE182B-CA28-43A4-8BC3-90ADADE2CD3E}"/>
+    <workbookView xWindow="13152" yWindow="7104" windowWidth="23040" windowHeight="17544" xr2:uid="{84DE182B-CA28-43A4-8BC3-90ADADE2CD3E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="57">
   <si>
     <t>Test Name</t>
   </si>
@@ -53,21 +53,176 @@
     <t>Login</t>
   </si>
   <si>
-    <t>Data validation</t>
-  </si>
-  <si>
     <t>No check to prevent multiple logins</t>
   </si>
   <si>
     <t>No restriction for admin-only transactions with standard login</t>
+  </si>
+  <si>
+    <t>Logout</t>
+  </si>
+  <si>
+    <t>No check to prevent logout if not logged in</t>
+  </si>
+  <si>
+    <t>Withdraw</t>
+  </si>
+  <si>
+    <t>Does not verify if the account exists</t>
+  </si>
+  <si>
+    <t>Does not enforce a withdraw limit of $500</t>
+  </si>
+  <si>
+    <t>Does not check if withdrawal will result in a negative balance</t>
+  </si>
+  <si>
+    <t>Transfer</t>
+  </si>
+  <si>
+    <t>Does not check if both accounts exist</t>
+  </si>
+  <si>
+    <t>Does not check if the origin account belongs to the logged in user</t>
+  </si>
+  <si>
+    <t>Does not enforce a transfer limit of $1000</t>
+  </si>
+  <si>
+    <t>Does not check if the origin account has sufficient funds</t>
+  </si>
+  <si>
+    <t>Paybill</t>
+  </si>
+  <si>
+    <t>Does not check if the account exists</t>
+  </si>
+  <si>
+    <t>Does not enforce a bill limit of $2000</t>
+  </si>
+  <si>
+    <t>Does not check if the account has sufficient funds</t>
+  </si>
+  <si>
+    <t>Deposit</t>
+  </si>
+  <si>
+    <t>02_login_invalid_multiple_logins</t>
+  </si>
+  <si>
+    <t>02_login_invalid_admin_only</t>
+  </si>
+  <si>
+    <t>Create</t>
+  </si>
+  <si>
+    <t>Does not restrict use of create to admin accounts</t>
+  </si>
+  <si>
+    <t>Does not limit account names to 20 characters</t>
+  </si>
+  <si>
+    <t>Does not enforce an initial balance limit of $99,999.99</t>
+  </si>
+  <si>
+    <t>Delete</t>
+  </si>
+  <si>
+    <t>02_login_invalid_logout.txt</t>
+  </si>
+  <si>
+    <t>03_withdraw_invalid_no_account.txt</t>
+  </si>
+  <si>
+    <t>03_withdraw_invalid_no_limit.txt</t>
+  </si>
+  <si>
+    <t>03_withdraw_invalid_negative.txt</t>
+  </si>
+  <si>
+    <t>04_transfer_invalid_no_accounts.txt</t>
+  </si>
+  <si>
+    <t>04_transfer_invalid_diff_origin.txt</t>
+  </si>
+  <si>
+    <t>04_transfer_invalid_no_limit.txt</t>
+  </si>
+  <si>
+    <t>04_transfer_invalid_sufficient.txt</t>
+  </si>
+  <si>
+    <t>05_paybill_invalid_no_account.txt</t>
+  </si>
+  <si>
+    <t>05_paybill_invalid_no_limit.txt</t>
+  </si>
+  <si>
+    <t>05_paybill_invalid_sufficient.txt</t>
+  </si>
+  <si>
+    <t>06_deposit_invalid_no_account.txt</t>
+  </si>
+  <si>
+    <t>01_create_invalid_no_admin.txt</t>
+  </si>
+  <si>
+    <t>01_create_invalid_char_limit.txt</t>
+  </si>
+  <si>
+    <t>01_create_invalid_bal_limit.txt</t>
+  </si>
+  <si>
+    <t>09_delete_invalid_no_admin.txt</t>
+  </si>
+  <si>
+    <t>09_delete_invalid_no_account.txt</t>
+  </si>
+  <si>
+    <t>Disable</t>
+  </si>
+  <si>
+    <t>08_disable_invalid_no_admin.txt</t>
+  </si>
+  <si>
+    <t>Does not restrict use of delete to admin accounts</t>
+  </si>
+  <si>
+    <t>Does not restrict use of disable to admin accounts</t>
+  </si>
+  <si>
+    <t>Changeplan</t>
+  </si>
+  <si>
+    <t>08_disable_invalid_no_account.txt</t>
+  </si>
+  <si>
+    <t>Does not restrict use of changeplan to admin accounts</t>
+  </si>
+  <si>
+    <t>07_changeplan_invalid_no_admin.txt</t>
+  </si>
+  <si>
+    <t>07_changeplan_invalid_no_account.txt</t>
+  </si>
+  <si>
+    <t>Data validation - if/else chain and while loop</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
@@ -95,8 +250,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -112,6 +268,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -431,60 +591,355 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78A7481D-5A8F-4A12-81BF-F0F307BBE9C7}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.77734375" customWidth="1"/>
+    <col min="1" max="1" width="32.21875" customWidth="1"/>
     <col min="2" max="2" width="17.88671875" customWidth="1"/>
-    <col min="3" max="3" width="49.21875" customWidth="1"/>
-    <col min="4" max="4" width="27.88671875" customWidth="1"/>
+    <col min="3" max="3" width="52.5546875" customWidth="1"/>
+    <col min="4" max="4" width="42.109375" customWidth="1"/>
     <col min="5" max="5" width="14.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>23</v>
+      </c>
       <c r="B2" t="s">
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>5</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>24</v>
+      </c>
       <c r="B3" t="s">
         <v>4</v>
       </c>
       <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" t="s">
         <v>7</v>
       </c>
-      <c r="D3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B4" t="s">
-        <v>4</v>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>37</v>
+      </c>
+      <c r="B11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>38</v>
+      </c>
+      <c r="B12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>39</v>
+      </c>
+      <c r="B13" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" t="s">
+        <v>20</v>
+      </c>
+      <c r="D13" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>40</v>
+      </c>
+      <c r="B14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" t="s">
+        <v>21</v>
+      </c>
+      <c r="D14" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>41</v>
+      </c>
+      <c r="B15" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15" t="s">
+        <v>19</v>
+      </c>
+      <c r="D15" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>42</v>
+      </c>
+      <c r="B16" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16" t="s">
+        <v>26</v>
+      </c>
+      <c r="D16" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>43</v>
+      </c>
+      <c r="B17" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17" t="s">
+        <v>27</v>
+      </c>
+      <c r="D17" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>44</v>
+      </c>
+      <c r="B18" t="s">
+        <v>25</v>
+      </c>
+      <c r="C18" t="s">
+        <v>28</v>
+      </c>
+      <c r="D18" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>45</v>
+      </c>
+      <c r="B19" t="s">
+        <v>29</v>
+      </c>
+      <c r="C19" t="s">
+        <v>49</v>
+      </c>
+      <c r="D19" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>46</v>
+      </c>
+      <c r="B20" t="s">
+        <v>29</v>
+      </c>
+      <c r="C20" t="s">
+        <v>19</v>
+      </c>
+      <c r="D20" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>48</v>
+      </c>
+      <c r="B21" t="s">
+        <v>47</v>
+      </c>
+      <c r="C21" t="s">
+        <v>50</v>
+      </c>
+      <c r="D21" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>52</v>
+      </c>
+      <c r="B22" t="s">
+        <v>47</v>
+      </c>
+      <c r="C22" t="s">
+        <v>19</v>
+      </c>
+      <c r="D22" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>54</v>
+      </c>
+      <c r="B23" t="s">
+        <v>51</v>
+      </c>
+      <c r="C23" t="s">
+        <v>53</v>
+      </c>
+      <c r="D23" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>55</v>
+      </c>
+      <c r="B24" t="s">
+        <v>51</v>
+      </c>
+      <c r="C24" t="s">
+        <v>19</v>
+      </c>
+      <c r="D24" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added more detailed failure solution descriptions
</commit_message>
<xml_diff>
--- a/FailureTable.xlsx
+++ b/FailureTable.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4d965ff5125c3e04/University/Year 1 Sem 2/Software QA/SQA Project/SQA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="134" documentId="8_{1A19906C-396F-4516-B957-E8AC86749972}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{34678FBE-2C41-4E9A-BE12-E11B5E1DF877}"/>
+  <xr:revisionPtr revIDLastSave="161" documentId="8_{1A19906C-396F-4516-B957-E8AC86749972}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4D2C133D-8B58-48CE-ACAD-1D4D9F6714C1}"/>
   <bookViews>
-    <workbookView xWindow="13152" yWindow="7104" windowWidth="23040" windowHeight="17544" xr2:uid="{84DE182B-CA28-43A4-8BC3-90ADADE2CD3E}"/>
+    <workbookView xWindow="6852" yWindow="2412" windowWidth="23040" windowHeight="16680" xr2:uid="{84DE182B-CA28-43A4-8BC3-90ADADE2CD3E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="79">
   <si>
     <t>Test Name</t>
   </si>
@@ -206,7 +206,73 @@
     <t>07_changeplan_invalid_no_account.txt</t>
   </si>
   <si>
-    <t>Data validation - if/else chain and while loop</t>
+    <t>Added a session check to prevent logging in while already logged in</t>
+  </si>
+  <si>
+    <t>Enforced admin privilege checks before executing admin-specific transactions</t>
+  </si>
+  <si>
+    <t>Added a session check to prevent logout when no session is active</t>
+  </si>
+  <si>
+    <t>Implemented a check to ensure an account is associated with the session before withdrawing</t>
+  </si>
+  <si>
+    <t>Restricted withdrawal amount to a maximum of $500 using get_valid_number_input()</t>
+  </si>
+  <si>
+    <t>Added a loop that prevents withdrawals exceeding the available balance</t>
+  </si>
+  <si>
+    <t>Implemented checks for both sender and receiver accounts before proceeding</t>
+  </si>
+  <si>
+    <t>Ensured that the sender account matches the current session's account</t>
+  </si>
+  <si>
+    <t>Restricted transfer amount to a maximum of $1000 using get_valid_number_input()</t>
+  </si>
+  <si>
+    <t>Added a loop that prevents transfers exceeding the sender's balance</t>
+  </si>
+  <si>
+    <t>Implemented a check to ensure an account is associated with the session before paying bills</t>
+  </si>
+  <si>
+    <t>Restricted bill payment amount to a maximum of $2000 using get_valid_number_input()</t>
+  </si>
+  <si>
+    <t>Added a loop that prevents bill payments exceeding the account balance</t>
+  </si>
+  <si>
+    <t>Implemented a check to ensure an account is associated with the session before depositing</t>
+  </si>
+  <si>
+    <t>Enforced admin privilege checks before allowing account creation</t>
+  </si>
+  <si>
+    <t>Added a check to ensure account names do not exceed 20 characters</t>
+  </si>
+  <si>
+    <t>Restricted the initial balance input to a maximum of $99,999.99 using get_valid_number_input()</t>
+  </si>
+  <si>
+    <t>Enforced admin privilege checks before allowing account deletion</t>
+  </si>
+  <si>
+    <t>Implemented a check to ensure the account exists before deletion</t>
+  </si>
+  <si>
+    <t>Enforced admin privilege checks before allowing account disabling</t>
+  </si>
+  <si>
+    <t>Implemented a check to ensure the account exists before disabling</t>
+  </si>
+  <si>
+    <t>Enforced admin privilege checks before allowing plan changes</t>
+  </si>
+  <si>
+    <t>Implemented a check to ensure the account exists before changing the plan</t>
   </si>
 </sst>
 </file>
@@ -594,7 +660,7 @@
   <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -602,7 +668,7 @@
     <col min="1" max="1" width="32.21875" customWidth="1"/>
     <col min="2" max="2" width="17.88671875" customWidth="1"/>
     <col min="3" max="3" width="52.5546875" customWidth="1"/>
-    <col min="4" max="4" width="42.109375" customWidth="1"/>
+    <col min="4" max="4" width="79.109375" customWidth="1"/>
     <col min="5" max="5" width="14.109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -645,7 +711,7 @@
         <v>6</v>
       </c>
       <c r="D3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -659,7 +725,7 @@
         <v>8</v>
       </c>
       <c r="D4" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -673,7 +739,7 @@
         <v>10</v>
       </c>
       <c r="D5" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -687,7 +753,7 @@
         <v>11</v>
       </c>
       <c r="D6" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -701,7 +767,7 @@
         <v>12</v>
       </c>
       <c r="D7" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -715,7 +781,7 @@
         <v>14</v>
       </c>
       <c r="D8" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -729,7 +795,7 @@
         <v>15</v>
       </c>
       <c r="D9" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
@@ -743,7 +809,7 @@
         <v>16</v>
       </c>
       <c r="D10" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
@@ -757,7 +823,7 @@
         <v>17</v>
       </c>
       <c r="D11" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
@@ -771,7 +837,7 @@
         <v>19</v>
       </c>
       <c r="D12" t="s">
-        <v>56</v>
+        <v>66</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
@@ -785,7 +851,7 @@
         <v>20</v>
       </c>
       <c r="D13" t="s">
-        <v>56</v>
+        <v>67</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -799,7 +865,7 @@
         <v>21</v>
       </c>
       <c r="D14" t="s">
-        <v>56</v>
+        <v>68</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
@@ -813,7 +879,7 @@
         <v>19</v>
       </c>
       <c r="D15" t="s">
-        <v>56</v>
+        <v>69</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
@@ -827,7 +893,7 @@
         <v>26</v>
       </c>
       <c r="D16" t="s">
-        <v>56</v>
+        <v>70</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
@@ -841,7 +907,7 @@
         <v>27</v>
       </c>
       <c r="D17" t="s">
-        <v>56</v>
+        <v>71</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
@@ -855,7 +921,7 @@
         <v>28</v>
       </c>
       <c r="D18" t="s">
-        <v>56</v>
+        <v>72</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
@@ -869,7 +935,7 @@
         <v>49</v>
       </c>
       <c r="D19" t="s">
-        <v>56</v>
+        <v>73</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
@@ -883,7 +949,7 @@
         <v>19</v>
       </c>
       <c r="D20" t="s">
-        <v>56</v>
+        <v>74</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
@@ -897,7 +963,7 @@
         <v>50</v>
       </c>
       <c r="D21" t="s">
-        <v>56</v>
+        <v>75</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
@@ -911,7 +977,7 @@
         <v>19</v>
       </c>
       <c r="D22" t="s">
-        <v>56</v>
+        <v>76</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
@@ -925,7 +991,7 @@
         <v>53</v>
       </c>
       <c r="D23" t="s">
-        <v>56</v>
+        <v>77</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
@@ -939,7 +1005,7 @@
         <v>19</v>
       </c>
       <c r="D24" t="s">
-        <v>56</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>